<commit_message>
Actualizamos template parser para que interprete reference_id. Todos los tests en verde, pero el campo no esta en la columna "A" sino en la "D".
</commit_message>
<xml_diff>
--- a/test/fixtures/files/mixed-sizes.xlsx
+++ b/test/fixtures/files/mixed-sizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiralles/Projects/stash/5411-IM-API/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A311AA4F-E19F-264B-8A94-4B3322F1294C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBD1BE9-013E-EE40-A8B7-B9FAE60EEA83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32140" yWindow="2460" windowWidth="26600" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31000" yWindow="2460" windowWidth="26600" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template Modelo" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
   <si>
     <t>BOX</t>
   </si>
@@ -181,6 +181,9 @@
   <si>
     <t>34</t>
     <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>REFERENCE_ID</t>
   </si>
 </sst>
 </file>
@@ -1725,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:V14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1736,9 +1739,10 @@
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>23</v>
       </c>
@@ -1749,61 +1753,64 @@
         <v>2</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="F1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="O1" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="32" t="s">
+      <c r="P1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="Q1" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="R1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="32" t="s">
+      <c r="S1" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="T1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="U1" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="32" t="s">
+      <c r="V1" s="32" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="16">
         <v>23694</v>
       </c>
@@ -1813,13 +1820,13 @@
       <c r="C2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="16"/>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
-      <c r="J2" s="22"/>
+      <c r="J2" s="21"/>
       <c r="K2" s="22"/>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
@@ -1827,16 +1834,17 @@
       <c r="O2" s="22"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
-      <c r="R2" s="22">
+      <c r="R2" s="22"/>
+      <c r="S2" s="22">
         <v>1</v>
       </c>
-      <c r="S2" s="22"/>
       <c r="T2" s="22"/>
-      <c r="U2" s="22">
+      <c r="U2" s="22"/>
+      <c r="V2" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="16">
         <v>23695</v>
       </c>
@@ -1846,23 +1854,23 @@
       <c r="C3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="23">
+      <c r="D3" s="16"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="23">
         <v>7</v>
       </c>
-      <c r="F3" s="21">
+      <c r="G3" s="21">
         <v>14</v>
       </c>
-      <c r="G3" s="21">
+      <c r="H3" s="21">
         <v>11</v>
       </c>
-      <c r="H3" s="21">
+      <c r="I3" s="21">
         <v>8</v>
       </c>
-      <c r="I3" s="21">
+      <c r="J3" s="21">
         <v>2</v>
       </c>
-      <c r="J3" s="22"/>
       <c r="K3" s="22"/>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
@@ -1874,8 +1882,9 @@
       <c r="S3" s="22"/>
       <c r="T3" s="22"/>
       <c r="U3" s="22"/>
-    </row>
-    <row r="4" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V3" s="22"/>
+    </row>
+    <row r="4" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17">
         <v>21370</v>
       </c>
@@ -1891,42 +1900,43 @@
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="21">
+      <c r="J4" s="17"/>
+      <c r="K4" s="21">
         <v>8</v>
       </c>
-      <c r="K4" s="21">
+      <c r="L4" s="21">
         <v>11</v>
       </c>
-      <c r="L4" s="21">
+      <c r="M4" s="21">
         <v>18</v>
       </c>
-      <c r="M4" s="21">
+      <c r="N4" s="21">
         <v>21</v>
       </c>
-      <c r="N4" s="21">
+      <c r="O4" s="21">
         <v>24</v>
       </c>
-      <c r="O4" s="21">
+      <c r="P4" s="21">
         <v>26</v>
       </c>
-      <c r="P4" s="21">
+      <c r="Q4" s="21">
         <v>18</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="R4" s="21">
         <v>12</v>
       </c>
-      <c r="R4" s="21">
+      <c r="S4" s="21">
         <v>13</v>
       </c>
-      <c r="S4" s="21">
+      <c r="T4" s="21">
         <v>12</v>
       </c>
-      <c r="T4" s="21">
+      <c r="U4" s="21">
         <v>13</v>
       </c>
-      <c r="U4" s="21"/>
-    </row>
-    <row r="5" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V4" s="21"/>
+    </row>
+    <row r="5" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="18">
         <v>20343</v>
       </c>
@@ -1936,30 +1946,31 @@
       <c r="C5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
-      <c r="J5" s="24"/>
+      <c r="J5" s="17"/>
       <c r="K5" s="24"/>
       <c r="L5" s="24"/>
-      <c r="M5" s="24">
-        <v>1</v>
-      </c>
+      <c r="M5" s="24"/>
       <c r="N5" s="24">
         <v>1</v>
       </c>
-      <c r="O5" s="24"/>
+      <c r="O5" s="24">
+        <v>1</v>
+      </c>
       <c r="P5" s="24"/>
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
-    </row>
-    <row r="6" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V5" s="24"/>
+    </row>
+    <row r="6" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="18">
         <v>23925</v>
       </c>
@@ -1969,50 +1980,51 @@
       <c r="C6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
-      <c r="J6" s="24">
+      <c r="J6" s="17"/>
+      <c r="K6" s="24">
         <v>2</v>
       </c>
-      <c r="K6" s="24">
+      <c r="L6" s="24">
         <v>7</v>
-      </c>
-      <c r="L6" s="24">
-        <v>15</v>
       </c>
       <c r="M6" s="24">
         <v>15</v>
       </c>
       <c r="N6" s="24">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O6" s="24">
         <v>16</v>
       </c>
       <c r="P6" s="24">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="24">
         <v>12</v>
       </c>
-      <c r="Q6" s="24">
+      <c r="R6" s="24">
         <v>7</v>
       </c>
-      <c r="R6" s="24">
+      <c r="S6" s="24">
         <v>4</v>
-      </c>
-      <c r="S6" s="24">
-        <v>2</v>
       </c>
       <c r="T6" s="24">
         <v>2</v>
       </c>
       <c r="U6" s="24">
+        <v>2</v>
+      </c>
+      <c r="V6" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="18">
         <v>23926</v>
       </c>
@@ -2022,46 +2034,47 @@
       <c r="C7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
-      <c r="J7" s="24">
+      <c r="J7" s="17"/>
+      <c r="K7" s="24">
         <v>4</v>
       </c>
-      <c r="K7" s="24">
+      <c r="L7" s="24">
         <v>5</v>
       </c>
-      <c r="L7" s="24">
+      <c r="M7" s="24">
         <v>13</v>
       </c>
-      <c r="M7" s="24">
+      <c r="N7" s="24">
         <v>20</v>
-      </c>
-      <c r="N7" s="24">
-        <v>21</v>
       </c>
       <c r="O7" s="24">
         <v>21</v>
       </c>
       <c r="P7" s="24">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="24">
         <v>19</v>
       </c>
-      <c r="Q7" s="24">
+      <c r="R7" s="24">
         <v>8</v>
       </c>
-      <c r="R7" s="24">
+      <c r="S7" s="24">
         <v>5</v>
       </c>
-      <c r="S7" s="24">
+      <c r="T7" s="24">
         <v>4</v>
       </c>
-      <c r="T7" s="24"/>
       <c r="U7" s="24"/>
-    </row>
-    <row r="8" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V7" s="24"/>
+    </row>
+    <row r="8" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="18">
         <v>23928</v>
       </c>
@@ -2071,32 +2084,33 @@
       <c r="C8" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
-      <c r="J8" s="24"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="24"/>
-      <c r="L8" s="24">
-        <v>1</v>
-      </c>
+      <c r="L8" s="24"/>
       <c r="M8" s="24">
         <v>1</v>
       </c>
       <c r="N8" s="24">
         <v>1</v>
       </c>
-      <c r="O8" s="24"/>
+      <c r="O8" s="24">
+        <v>1</v>
+      </c>
       <c r="P8" s="24"/>
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
       <c r="S8" s="24"/>
       <c r="T8" s="24"/>
       <c r="U8" s="24"/>
-    </row>
-    <row r="9" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V8" s="24"/>
+    </row>
+    <row r="9" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="19">
         <v>23607</v>
       </c>
@@ -2106,16 +2120,14 @@
       <c r="C9" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="26"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27">
-        <v>1</v>
-      </c>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
       <c r="L9" s="27">
         <v>1</v>
       </c>
@@ -2125,15 +2137,18 @@
       <c r="N9" s="27">
         <v>1</v>
       </c>
-      <c r="O9" s="27"/>
+      <c r="O9" s="27">
+        <v>1</v>
+      </c>
       <c r="P9" s="27"/>
       <c r="Q9" s="27"/>
       <c r="R9" s="27"/>
-      <c r="S9" s="28"/>
+      <c r="S9" s="27"/>
       <c r="T9" s="28"/>
-      <c r="U9" s="29"/>
-    </row>
-    <row r="10" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="U9" s="28"/>
+      <c r="V9" s="29"/>
+    </row>
+    <row r="10" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="19">
         <v>23180</v>
       </c>
@@ -2143,25 +2158,25 @@
       <c r="C10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="19"/>
+      <c r="E10" s="28">
         <v>41</v>
       </c>
-      <c r="E10" s="28">
+      <c r="F10" s="28">
         <v>87</v>
       </c>
-      <c r="F10" s="28">
+      <c r="G10" s="28">
         <v>115</v>
       </c>
-      <c r="G10" s="28">
+      <c r="H10" s="28">
         <v>74</v>
       </c>
-      <c r="H10" s="28">
+      <c r="I10" s="28">
         <v>41</v>
       </c>
-      <c r="I10" s="28">
+      <c r="J10" s="28">
         <v>9</v>
       </c>
-      <c r="J10" s="28"/>
       <c r="K10" s="28"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
@@ -2172,9 +2187,10 @@
       <c r="R10" s="28"/>
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
-      <c r="U10" s="29"/>
-    </row>
-    <row r="11" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="U10" s="28"/>
+      <c r="V10" s="29"/>
+    </row>
+    <row r="11" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="19">
         <v>23608</v>
       </c>
@@ -2184,46 +2200,47 @@
       <c r="C11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
-      <c r="J11" s="28">
+      <c r="J11" s="28"/>
+      <c r="K11" s="28">
         <v>10</v>
       </c>
-      <c r="K11" s="28">
+      <c r="L11" s="28">
         <v>12</v>
       </c>
-      <c r="L11" s="28">
+      <c r="M11" s="28">
         <v>19</v>
-      </c>
-      <c r="M11" s="28">
-        <v>25</v>
       </c>
       <c r="N11" s="28">
         <v>25</v>
       </c>
       <c r="O11" s="28">
+        <v>25</v>
+      </c>
+      <c r="P11" s="28">
         <v>23</v>
       </c>
-      <c r="P11" s="28">
+      <c r="Q11" s="28">
         <v>20</v>
       </c>
-      <c r="Q11" s="28">
+      <c r="R11" s="28">
         <v>10</v>
       </c>
-      <c r="R11" s="28">
+      <c r="S11" s="28">
         <v>5</v>
       </c>
-      <c r="S11" s="28">
+      <c r="T11" s="28">
         <v>4</v>
       </c>
-      <c r="T11" s="28"/>
       <c r="U11" s="28"/>
-    </row>
-    <row r="12" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V11" s="28"/>
+    </row>
+    <row r="12" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="19">
         <v>23173</v>
       </c>
@@ -2233,23 +2250,21 @@
       <c r="C12" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
-      <c r="J12" s="28">
+      <c r="J12" s="28"/>
+      <c r="K12" s="28">
         <v>2</v>
       </c>
-      <c r="K12" s="28">
+      <c r="L12" s="28">
         <v>4</v>
       </c>
-      <c r="L12" s="28">
+      <c r="M12" s="28">
         <v>14</v>
-      </c>
-      <c r="M12" s="28">
-        <v>17</v>
       </c>
       <c r="N12" s="28">
         <v>17</v>
@@ -2258,25 +2273,28 @@
         <v>17</v>
       </c>
       <c r="P12" s="28">
+        <v>17</v>
+      </c>
+      <c r="Q12" s="28">
         <v>12</v>
       </c>
-      <c r="Q12" s="28">
+      <c r="R12" s="28">
         <v>7</v>
       </c>
-      <c r="R12" s="28">
+      <c r="S12" s="28">
         <v>5</v>
-      </c>
-      <c r="S12" s="28">
-        <v>3</v>
       </c>
       <c r="T12" s="28">
         <v>3</v>
       </c>
       <c r="U12" s="28">
+        <v>3</v>
+      </c>
+      <c r="V12" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="19">
         <v>23233</v>
       </c>
@@ -2286,48 +2304,49 @@
       <c r="C13" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
-      <c r="J13" s="28">
+      <c r="J13" s="28"/>
+      <c r="K13" s="28">
         <v>3</v>
       </c>
-      <c r="K13" s="28">
+      <c r="L13" s="28">
         <v>4</v>
       </c>
-      <c r="L13" s="28">
+      <c r="M13" s="28">
         <v>10</v>
       </c>
-      <c r="M13" s="28">
+      <c r="N13" s="28">
         <v>15</v>
       </c>
-      <c r="N13" s="30">
+      <c r="O13" s="30">
         <v>17</v>
       </c>
-      <c r="O13" s="28">
+      <c r="P13" s="28">
         <v>16</v>
       </c>
-      <c r="P13" s="28">
+      <c r="Q13" s="28">
         <v>14</v>
       </c>
-      <c r="Q13" s="28">
+      <c r="R13" s="28">
         <v>7</v>
       </c>
-      <c r="R13" s="28">
+      <c r="S13" s="28">
         <v>5</v>
       </c>
-      <c r="S13" s="28">
+      <c r="T13" s="28">
         <v>3</v>
       </c>
-      <c r="T13" s="28">
+      <c r="U13" s="28">
         <v>1</v>
       </c>
-      <c r="U13" s="28"/>
-    </row>
-    <row r="14" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V13" s="28"/>
+    </row>
+    <row r="14" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="19">
         <v>23178</v>
       </c>
@@ -2337,44 +2356,45 @@
       <c r="C14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
-      <c r="K14" s="28">
+      <c r="K14" s="28"/>
+      <c r="L14" s="28">
         <v>1</v>
       </c>
-      <c r="L14" s="28">
+      <c r="M14" s="28">
         <v>6</v>
       </c>
-      <c r="M14" s="28">
+      <c r="N14" s="28">
         <v>8</v>
       </c>
-      <c r="N14" s="28">
+      <c r="O14" s="28">
         <v>12</v>
       </c>
-      <c r="O14" s="28">
+      <c r="P14" s="28">
         <v>14</v>
       </c>
-      <c r="P14" s="28">
+      <c r="Q14" s="28">
         <v>12</v>
       </c>
-      <c r="Q14" s="28">
+      <c r="R14" s="28">
         <v>8</v>
       </c>
-      <c r="R14" s="28">
+      <c r="S14" s="28">
         <v>6</v>
       </c>
-      <c r="S14" s="28">
+      <c r="T14" s="28">
         <v>5</v>
       </c>
-      <c r="T14" s="28">
+      <c r="U14" s="28">
         <v>3</v>
       </c>
-      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se agrego box_id a las transacciones de stock.
# Se creo una migracion en la cual se agrega box_id al schema de
#    stock_transactions.
#
# Se agrego box_id a las transacciones de stock.
#
# Se modificaron los archivos xlsx de los test agregando dicho campo.
#    (los archivos afectados son mixed-sizes, pl_beamount_organic,
#     tpl).
#
# Se elimino el archivo pl_reference_id_only y se agrego el archivo
#    "pl_reference_id_and_box_id".
#
# Se unifico el test "can parse reference_id only" con
#    "can parse reference_id and box_id" para testear los dos campos
#    con el mismo test.
#
# Se modificaron las coordenadas de las columnas de los xlsx
# para que los talles arranquen en la columna "F".
</commit_message>
<xml_diff>
--- a/test/fixtures/files/mixed-sizes.xlsx
+++ b/test/fixtures/files/mixed-sizes.xlsx
@@ -5,18 +5,18 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiralles/Projects/stash/5411-IM-API/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonatansteckler/dev/stash/5411-IM-API/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBD1BE9-013E-EE40-A8B7-B9FAE60EEA83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6E62FA-B42F-7743-8603-1DEBF9B19DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31000" yWindow="2460" windowWidth="26600" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template Modelo" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja 1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>BOX</t>
   </si>
@@ -570,8 +570,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="3" xr:uid="{A36ED469-7401-3E49-AF43-EA460355A6BD}"/>
   </cellStyles>
@@ -1728,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1739,10 +1739,10 @@
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="4" max="5" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>23</v>
       </c>
@@ -1756,61 +1756,64 @@
         <v>48</v>
       </c>
       <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="K1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="O1" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="32" t="s">
+      <c r="P1" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="Q1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="R1" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="32" t="s">
+      <c r="S1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="T1" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="U1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="32" t="s">
+      <c r="V1" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="32" t="s">
+      <c r="W1" s="32" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="16">
         <v>23694</v>
       </c>
@@ -1821,13 +1824,13 @@
         <v>30</v>
       </c>
       <c r="D2" s="16"/>
-      <c r="E2" s="21"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
-      <c r="K2" s="22"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
@@ -1835,16 +1838,17 @@
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
       <c r="R2" s="22"/>
-      <c r="S2" s="22">
+      <c r="S2" s="22"/>
+      <c r="T2" s="22">
         <v>1</v>
       </c>
-      <c r="T2" s="22"/>
       <c r="U2" s="22"/>
-      <c r="V2" s="22">
+      <c r="V2" s="22"/>
+      <c r="W2" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="16">
         <v>23695</v>
       </c>
@@ -1855,23 +1859,23 @@
         <v>31</v>
       </c>
       <c r="D3" s="16"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="23">
+      <c r="E3" s="16"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="23">
         <v>7</v>
       </c>
-      <c r="G3" s="21">
+      <c r="H3" s="21">
         <v>14</v>
       </c>
-      <c r="H3" s="21">
+      <c r="I3" s="21">
         <v>11</v>
       </c>
-      <c r="I3" s="21">
+      <c r="J3" s="21">
         <v>8</v>
       </c>
-      <c r="J3" s="21">
+      <c r="K3" s="21">
         <v>2</v>
       </c>
-      <c r="K3" s="22"/>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
@@ -1883,8 +1887,9 @@
       <c r="T3" s="22"/>
       <c r="U3" s="22"/>
       <c r="V3" s="22"/>
-    </row>
-    <row r="4" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W3" s="22"/>
+    </row>
+    <row r="4" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17">
         <v>21370</v>
       </c>
@@ -1901,42 +1906,43 @@
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="21">
+      <c r="K4" s="17"/>
+      <c r="L4" s="21">
         <v>8</v>
       </c>
-      <c r="L4" s="21">
+      <c r="M4" s="21">
         <v>11</v>
       </c>
-      <c r="M4" s="21">
+      <c r="N4" s="21">
         <v>18</v>
       </c>
-      <c r="N4" s="21">
+      <c r="O4" s="21">
         <v>21</v>
       </c>
-      <c r="O4" s="21">
+      <c r="P4" s="21">
         <v>24</v>
       </c>
-      <c r="P4" s="21">
+      <c r="Q4" s="21">
         <v>26</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="R4" s="21">
         <v>18</v>
       </c>
-      <c r="R4" s="21">
+      <c r="S4" s="21">
         <v>12</v>
       </c>
-      <c r="S4" s="21">
+      <c r="T4" s="21">
         <v>13</v>
       </c>
-      <c r="T4" s="21">
+      <c r="U4" s="21">
         <v>12</v>
       </c>
-      <c r="U4" s="21">
+      <c r="V4" s="21">
         <v>13</v>
       </c>
-      <c r="V4" s="21"/>
-    </row>
-    <row r="5" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W4" s="21"/>
+    </row>
+    <row r="5" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="18">
         <v>20343</v>
       </c>
@@ -1947,30 +1953,31 @@
         <v>33</v>
       </c>
       <c r="D5" s="20"/>
-      <c r="E5" s="17"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
-      <c r="K5" s="24"/>
+      <c r="K5" s="17"/>
       <c r="L5" s="24"/>
       <c r="M5" s="24"/>
-      <c r="N5" s="24">
-        <v>1</v>
-      </c>
+      <c r="N5" s="24"/>
       <c r="O5" s="24">
         <v>1</v>
       </c>
-      <c r="P5" s="24"/>
+      <c r="P5" s="24">
+        <v>1</v>
+      </c>
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
       <c r="V5" s="24"/>
-    </row>
-    <row r="6" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W5" s="24"/>
+    </row>
+    <row r="6" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="18">
         <v>23925</v>
       </c>
@@ -1981,50 +1988,51 @@
         <v>33</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="17"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
-      <c r="K6" s="24">
+      <c r="K6" s="17"/>
+      <c r="L6" s="24">
         <v>2</v>
       </c>
-      <c r="L6" s="24">
+      <c r="M6" s="24">
         <v>7</v>
-      </c>
-      <c r="M6" s="24">
-        <v>15</v>
       </c>
       <c r="N6" s="24">
         <v>15</v>
       </c>
       <c r="O6" s="24">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P6" s="24">
         <v>16</v>
       </c>
       <c r="Q6" s="24">
+        <v>16</v>
+      </c>
+      <c r="R6" s="24">
         <v>12</v>
       </c>
-      <c r="R6" s="24">
+      <c r="S6" s="24">
         <v>7</v>
       </c>
-      <c r="S6" s="24">
+      <c r="T6" s="24">
         <v>4</v>
-      </c>
-      <c r="T6" s="24">
-        <v>2</v>
       </c>
       <c r="U6" s="24">
         <v>2</v>
       </c>
       <c r="V6" s="24">
+        <v>2</v>
+      </c>
+      <c r="W6" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="18">
         <v>23926</v>
       </c>
@@ -2035,46 +2043,47 @@
         <v>33</v>
       </c>
       <c r="D7" s="20"/>
-      <c r="E7" s="17"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
-      <c r="K7" s="24">
+      <c r="K7" s="17"/>
+      <c r="L7" s="24">
         <v>4</v>
       </c>
-      <c r="L7" s="24">
+      <c r="M7" s="24">
         <v>5</v>
       </c>
-      <c r="M7" s="24">
+      <c r="N7" s="24">
         <v>13</v>
       </c>
-      <c r="N7" s="24">
+      <c r="O7" s="24">
         <v>20</v>
-      </c>
-      <c r="O7" s="24">
-        <v>21</v>
       </c>
       <c r="P7" s="24">
         <v>21</v>
       </c>
       <c r="Q7" s="24">
+        <v>21</v>
+      </c>
+      <c r="R7" s="24">
         <v>19</v>
       </c>
-      <c r="R7" s="24">
+      <c r="S7" s="24">
         <v>8</v>
       </c>
-      <c r="S7" s="24">
+      <c r="T7" s="24">
         <v>5</v>
       </c>
-      <c r="T7" s="24">
+      <c r="U7" s="24">
         <v>4</v>
       </c>
-      <c r="U7" s="24"/>
       <c r="V7" s="24"/>
-    </row>
-    <row r="8" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W7" s="24"/>
+    </row>
+    <row r="8" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="18">
         <v>23928</v>
       </c>
@@ -2085,32 +2094,33 @@
         <v>33</v>
       </c>
       <c r="D8" s="20"/>
-      <c r="E8" s="25"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
-      <c r="K8" s="24"/>
+      <c r="K8" s="25"/>
       <c r="L8" s="24"/>
-      <c r="M8" s="24">
-        <v>1</v>
-      </c>
+      <c r="M8" s="24"/>
       <c r="N8" s="24">
         <v>1</v>
       </c>
       <c r="O8" s="24">
         <v>1</v>
       </c>
-      <c r="P8" s="24"/>
+      <c r="P8" s="24">
+        <v>1</v>
+      </c>
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
       <c r="S8" s="24"/>
       <c r="T8" s="24"/>
       <c r="U8" s="24"/>
       <c r="V8" s="24"/>
-    </row>
-    <row r="9" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W8" s="24"/>
+    </row>
+    <row r="9" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="19">
         <v>23607</v>
       </c>
@@ -2121,16 +2131,14 @@
         <v>34</v>
       </c>
       <c r="D9" s="19"/>
-      <c r="E9" s="26"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27">
-        <v>1</v>
-      </c>
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
       <c r="M9" s="27">
         <v>1</v>
       </c>
@@ -2140,15 +2148,18 @@
       <c r="O9" s="27">
         <v>1</v>
       </c>
-      <c r="P9" s="27"/>
+      <c r="P9" s="27">
+        <v>1</v>
+      </c>
       <c r="Q9" s="27"/>
       <c r="R9" s="27"/>
       <c r="S9" s="27"/>
-      <c r="T9" s="28"/>
+      <c r="T9" s="27"/>
       <c r="U9" s="28"/>
-      <c r="V9" s="29"/>
-    </row>
-    <row r="10" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="V9" s="28"/>
+      <c r="W9" s="29"/>
+    </row>
+    <row r="10" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="19">
         <v>23180</v>
       </c>
@@ -2159,25 +2170,25 @@
         <v>34</v>
       </c>
       <c r="D10" s="19"/>
-      <c r="E10" s="28">
+      <c r="E10" s="19"/>
+      <c r="F10" s="28">
         <v>41</v>
       </c>
-      <c r="F10" s="28">
+      <c r="G10" s="28">
         <v>87</v>
       </c>
-      <c r="G10" s="28">
+      <c r="H10" s="28">
         <v>115</v>
       </c>
-      <c r="H10" s="28">
+      <c r="I10" s="28">
         <v>74</v>
       </c>
-      <c r="I10" s="28">
+      <c r="J10" s="28">
         <v>41</v>
       </c>
-      <c r="J10" s="28">
+      <c r="K10" s="28">
         <v>9</v>
       </c>
-      <c r="K10" s="28"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -2188,9 +2199,10 @@
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
       <c r="U10" s="28"/>
-      <c r="V10" s="29"/>
-    </row>
-    <row r="11" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="V10" s="28"/>
+      <c r="W10" s="29"/>
+    </row>
+    <row r="11" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="19">
         <v>23608</v>
       </c>
@@ -2201,46 +2213,47 @@
         <v>34</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="28"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
-      <c r="K11" s="28">
+      <c r="K11" s="28"/>
+      <c r="L11" s="28">
         <v>10</v>
       </c>
-      <c r="L11" s="28">
+      <c r="M11" s="28">
         <v>12</v>
       </c>
-      <c r="M11" s="28">
+      <c r="N11" s="28">
         <v>19</v>
-      </c>
-      <c r="N11" s="28">
-        <v>25</v>
       </c>
       <c r="O11" s="28">
         <v>25</v>
       </c>
       <c r="P11" s="28">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="28">
         <v>23</v>
       </c>
-      <c r="Q11" s="28">
+      <c r="R11" s="28">
         <v>20</v>
       </c>
-      <c r="R11" s="28">
+      <c r="S11" s="28">
         <v>10</v>
       </c>
-      <c r="S11" s="28">
+      <c r="T11" s="28">
         <v>5</v>
       </c>
-      <c r="T11" s="28">
+      <c r="U11" s="28">
         <v>4</v>
       </c>
-      <c r="U11" s="28"/>
       <c r="V11" s="28"/>
-    </row>
-    <row r="12" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W11" s="28"/>
+    </row>
+    <row r="12" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="19">
         <v>23173</v>
       </c>
@@ -2251,23 +2264,21 @@
         <v>34</v>
       </c>
       <c r="D12" s="19"/>
-      <c r="E12" s="28"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
-      <c r="K12" s="28">
+      <c r="K12" s="28"/>
+      <c r="L12" s="28">
         <v>2</v>
       </c>
-      <c r="L12" s="28">
+      <c r="M12" s="28">
         <v>4</v>
       </c>
-      <c r="M12" s="28">
+      <c r="N12" s="28">
         <v>14</v>
-      </c>
-      <c r="N12" s="28">
-        <v>17</v>
       </c>
       <c r="O12" s="28">
         <v>17</v>
@@ -2276,25 +2287,28 @@
         <v>17</v>
       </c>
       <c r="Q12" s="28">
+        <v>17</v>
+      </c>
+      <c r="R12" s="28">
         <v>12</v>
       </c>
-      <c r="R12" s="28">
+      <c r="S12" s="28">
         <v>7</v>
       </c>
-      <c r="S12" s="28">
+      <c r="T12" s="28">
         <v>5</v>
-      </c>
-      <c r="T12" s="28">
-        <v>3</v>
       </c>
       <c r="U12" s="28">
         <v>3</v>
       </c>
       <c r="V12" s="28">
+        <v>3</v>
+      </c>
+      <c r="W12" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="19">
         <v>23233</v>
       </c>
@@ -2305,48 +2319,49 @@
         <v>34</v>
       </c>
       <c r="D13" s="19"/>
-      <c r="E13" s="28"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
-      <c r="K13" s="28">
+      <c r="K13" s="28"/>
+      <c r="L13" s="28">
         <v>3</v>
       </c>
-      <c r="L13" s="28">
+      <c r="M13" s="28">
         <v>4</v>
       </c>
-      <c r="M13" s="28">
+      <c r="N13" s="28">
         <v>10</v>
       </c>
-      <c r="N13" s="28">
+      <c r="O13" s="28">
         <v>15</v>
       </c>
-      <c r="O13" s="30">
+      <c r="P13" s="30">
         <v>17</v>
       </c>
-      <c r="P13" s="28">
+      <c r="Q13" s="28">
         <v>16</v>
       </c>
-      <c r="Q13" s="28">
+      <c r="R13" s="28">
         <v>14</v>
       </c>
-      <c r="R13" s="28">
+      <c r="S13" s="28">
         <v>7</v>
       </c>
-      <c r="S13" s="28">
+      <c r="T13" s="28">
         <v>5</v>
       </c>
-      <c r="T13" s="28">
+      <c r="U13" s="28">
         <v>3</v>
       </c>
-      <c r="U13" s="28">
+      <c r="V13" s="28">
         <v>1</v>
       </c>
-      <c r="V13" s="28"/>
-    </row>
-    <row r="14" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W13" s="28"/>
+    </row>
+    <row r="14" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="19">
         <v>23178</v>
       </c>
@@ -2357,44 +2372,45 @@
         <v>34</v>
       </c>
       <c r="D14" s="19"/>
-      <c r="E14" s="28"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
-      <c r="L14" s="28">
+      <c r="L14" s="28"/>
+      <c r="M14" s="28">
         <v>1</v>
       </c>
-      <c r="M14" s="28">
+      <c r="N14" s="28">
         <v>6</v>
       </c>
-      <c r="N14" s="28">
+      <c r="O14" s="28">
         <v>8</v>
       </c>
-      <c r="O14" s="28">
+      <c r="P14" s="28">
         <v>12</v>
       </c>
-      <c r="P14" s="28">
+      <c r="Q14" s="28">
         <v>14</v>
       </c>
-      <c r="Q14" s="28">
+      <c r="R14" s="28">
         <v>12</v>
       </c>
-      <c r="R14" s="28">
+      <c r="S14" s="28">
         <v>8</v>
       </c>
-      <c r="S14" s="28">
+      <c r="T14" s="28">
         <v>6</v>
       </c>
-      <c r="T14" s="28">
+      <c r="U14" s="28">
         <v>5</v>
       </c>
-      <c r="U14" s="28">
+      <c r="V14" s="28">
         <v>3</v>
       </c>
-      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se agrego box_id a las transacciones de stock. (#9)
Add refrence_id y box_id a las transacciones de stock
</commit_message>
<xml_diff>
--- a/test/fixtures/files/mixed-sizes.xlsx
+++ b/test/fixtures/files/mixed-sizes.xlsx
@@ -5,18 +5,18 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiralles/Projects/stash/5411-IM-API/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonatansteckler/dev/stash/5411-IM-API/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBD1BE9-013E-EE40-A8B7-B9FAE60EEA83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6E62FA-B42F-7743-8603-1DEBF9B19DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31000" yWindow="2460" windowWidth="26600" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template Modelo" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja 1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>BOX</t>
   </si>
@@ -570,8 +570,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="3" xr:uid="{A36ED469-7401-3E49-AF43-EA460355A6BD}"/>
   </cellStyles>
@@ -1728,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1739,10 +1739,10 @@
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="4" max="5" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>23</v>
       </c>
@@ -1756,61 +1756,64 @@
         <v>48</v>
       </c>
       <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="K1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="O1" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="32" t="s">
+      <c r="P1" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="Q1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="R1" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="32" t="s">
+      <c r="S1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="T1" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="U1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="32" t="s">
+      <c r="V1" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="32" t="s">
+      <c r="W1" s="32" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="16">
         <v>23694</v>
       </c>
@@ -1821,13 +1824,13 @@
         <v>30</v>
       </c>
       <c r="D2" s="16"/>
-      <c r="E2" s="21"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
-      <c r="K2" s="22"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
@@ -1835,16 +1838,17 @@
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
       <c r="R2" s="22"/>
-      <c r="S2" s="22">
+      <c r="S2" s="22"/>
+      <c r="T2" s="22">
         <v>1</v>
       </c>
-      <c r="T2" s="22"/>
       <c r="U2" s="22"/>
-      <c r="V2" s="22">
+      <c r="V2" s="22"/>
+      <c r="W2" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="16">
         <v>23695</v>
       </c>
@@ -1855,23 +1859,23 @@
         <v>31</v>
       </c>
       <c r="D3" s="16"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="23">
+      <c r="E3" s="16"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="23">
         <v>7</v>
       </c>
-      <c r="G3" s="21">
+      <c r="H3" s="21">
         <v>14</v>
       </c>
-      <c r="H3" s="21">
+      <c r="I3" s="21">
         <v>11</v>
       </c>
-      <c r="I3" s="21">
+      <c r="J3" s="21">
         <v>8</v>
       </c>
-      <c r="J3" s="21">
+      <c r="K3" s="21">
         <v>2</v>
       </c>
-      <c r="K3" s="22"/>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
@@ -1883,8 +1887,9 @@
       <c r="T3" s="22"/>
       <c r="U3" s="22"/>
       <c r="V3" s="22"/>
-    </row>
-    <row r="4" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W3" s="22"/>
+    </row>
+    <row r="4" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17">
         <v>21370</v>
       </c>
@@ -1901,42 +1906,43 @@
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="21">
+      <c r="K4" s="17"/>
+      <c r="L4" s="21">
         <v>8</v>
       </c>
-      <c r="L4" s="21">
+      <c r="M4" s="21">
         <v>11</v>
       </c>
-      <c r="M4" s="21">
+      <c r="N4" s="21">
         <v>18</v>
       </c>
-      <c r="N4" s="21">
+      <c r="O4" s="21">
         <v>21</v>
       </c>
-      <c r="O4" s="21">
+      <c r="P4" s="21">
         <v>24</v>
       </c>
-      <c r="P4" s="21">
+      <c r="Q4" s="21">
         <v>26</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="R4" s="21">
         <v>18</v>
       </c>
-      <c r="R4" s="21">
+      <c r="S4" s="21">
         <v>12</v>
       </c>
-      <c r="S4" s="21">
+      <c r="T4" s="21">
         <v>13</v>
       </c>
-      <c r="T4" s="21">
+      <c r="U4" s="21">
         <v>12</v>
       </c>
-      <c r="U4" s="21">
+      <c r="V4" s="21">
         <v>13</v>
       </c>
-      <c r="V4" s="21"/>
-    </row>
-    <row r="5" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W4" s="21"/>
+    </row>
+    <row r="5" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="18">
         <v>20343</v>
       </c>
@@ -1947,30 +1953,31 @@
         <v>33</v>
       </c>
       <c r="D5" s="20"/>
-      <c r="E5" s="17"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
-      <c r="K5" s="24"/>
+      <c r="K5" s="17"/>
       <c r="L5" s="24"/>
       <c r="M5" s="24"/>
-      <c r="N5" s="24">
-        <v>1</v>
-      </c>
+      <c r="N5" s="24"/>
       <c r="O5" s="24">
         <v>1</v>
       </c>
-      <c r="P5" s="24"/>
+      <c r="P5" s="24">
+        <v>1</v>
+      </c>
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
       <c r="V5" s="24"/>
-    </row>
-    <row r="6" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W5" s="24"/>
+    </row>
+    <row r="6" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="18">
         <v>23925</v>
       </c>
@@ -1981,50 +1988,51 @@
         <v>33</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="17"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
-      <c r="K6" s="24">
+      <c r="K6" s="17"/>
+      <c r="L6" s="24">
         <v>2</v>
       </c>
-      <c r="L6" s="24">
+      <c r="M6" s="24">
         <v>7</v>
-      </c>
-      <c r="M6" s="24">
-        <v>15</v>
       </c>
       <c r="N6" s="24">
         <v>15</v>
       </c>
       <c r="O6" s="24">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P6" s="24">
         <v>16</v>
       </c>
       <c r="Q6" s="24">
+        <v>16</v>
+      </c>
+      <c r="R6" s="24">
         <v>12</v>
       </c>
-      <c r="R6" s="24">
+      <c r="S6" s="24">
         <v>7</v>
       </c>
-      <c r="S6" s="24">
+      <c r="T6" s="24">
         <v>4</v>
-      </c>
-      <c r="T6" s="24">
-        <v>2</v>
       </c>
       <c r="U6" s="24">
         <v>2</v>
       </c>
       <c r="V6" s="24">
+        <v>2</v>
+      </c>
+      <c r="W6" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="18">
         <v>23926</v>
       </c>
@@ -2035,46 +2043,47 @@
         <v>33</v>
       </c>
       <c r="D7" s="20"/>
-      <c r="E7" s="17"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
-      <c r="K7" s="24">
+      <c r="K7" s="17"/>
+      <c r="L7" s="24">
         <v>4</v>
       </c>
-      <c r="L7" s="24">
+      <c r="M7" s="24">
         <v>5</v>
       </c>
-      <c r="M7" s="24">
+      <c r="N7" s="24">
         <v>13</v>
       </c>
-      <c r="N7" s="24">
+      <c r="O7" s="24">
         <v>20</v>
-      </c>
-      <c r="O7" s="24">
-        <v>21</v>
       </c>
       <c r="P7" s="24">
         <v>21</v>
       </c>
       <c r="Q7" s="24">
+        <v>21</v>
+      </c>
+      <c r="R7" s="24">
         <v>19</v>
       </c>
-      <c r="R7" s="24">
+      <c r="S7" s="24">
         <v>8</v>
       </c>
-      <c r="S7" s="24">
+      <c r="T7" s="24">
         <v>5</v>
       </c>
-      <c r="T7" s="24">
+      <c r="U7" s="24">
         <v>4</v>
       </c>
-      <c r="U7" s="24"/>
       <c r="V7" s="24"/>
-    </row>
-    <row r="8" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W7" s="24"/>
+    </row>
+    <row r="8" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="18">
         <v>23928</v>
       </c>
@@ -2085,32 +2094,33 @@
         <v>33</v>
       </c>
       <c r="D8" s="20"/>
-      <c r="E8" s="25"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
-      <c r="K8" s="24"/>
+      <c r="K8" s="25"/>
       <c r="L8" s="24"/>
-      <c r="M8" s="24">
-        <v>1</v>
-      </c>
+      <c r="M8" s="24"/>
       <c r="N8" s="24">
         <v>1</v>
       </c>
       <c r="O8" s="24">
         <v>1</v>
       </c>
-      <c r="P8" s="24"/>
+      <c r="P8" s="24">
+        <v>1</v>
+      </c>
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
       <c r="S8" s="24"/>
       <c r="T8" s="24"/>
       <c r="U8" s="24"/>
       <c r="V8" s="24"/>
-    </row>
-    <row r="9" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W8" s="24"/>
+    </row>
+    <row r="9" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="19">
         <v>23607</v>
       </c>
@@ -2121,16 +2131,14 @@
         <v>34</v>
       </c>
       <c r="D9" s="19"/>
-      <c r="E9" s="26"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27">
-        <v>1</v>
-      </c>
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
       <c r="M9" s="27">
         <v>1</v>
       </c>
@@ -2140,15 +2148,18 @@
       <c r="O9" s="27">
         <v>1</v>
       </c>
-      <c r="P9" s="27"/>
+      <c r="P9" s="27">
+        <v>1</v>
+      </c>
       <c r="Q9" s="27"/>
       <c r="R9" s="27"/>
       <c r="S9" s="27"/>
-      <c r="T9" s="28"/>
+      <c r="T9" s="27"/>
       <c r="U9" s="28"/>
-      <c r="V9" s="29"/>
-    </row>
-    <row r="10" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="V9" s="28"/>
+      <c r="W9" s="29"/>
+    </row>
+    <row r="10" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="19">
         <v>23180</v>
       </c>
@@ -2159,25 +2170,25 @@
         <v>34</v>
       </c>
       <c r="D10" s="19"/>
-      <c r="E10" s="28">
+      <c r="E10" s="19"/>
+      <c r="F10" s="28">
         <v>41</v>
       </c>
-      <c r="F10" s="28">
+      <c r="G10" s="28">
         <v>87</v>
       </c>
-      <c r="G10" s="28">
+      <c r="H10" s="28">
         <v>115</v>
       </c>
-      <c r="H10" s="28">
+      <c r="I10" s="28">
         <v>74</v>
       </c>
-      <c r="I10" s="28">
+      <c r="J10" s="28">
         <v>41</v>
       </c>
-      <c r="J10" s="28">
+      <c r="K10" s="28">
         <v>9</v>
       </c>
-      <c r="K10" s="28"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -2188,9 +2199,10 @@
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
       <c r="U10" s="28"/>
-      <c r="V10" s="29"/>
-    </row>
-    <row r="11" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="V10" s="28"/>
+      <c r="W10" s="29"/>
+    </row>
+    <row r="11" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="19">
         <v>23608</v>
       </c>
@@ -2201,46 +2213,47 @@
         <v>34</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="28"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
-      <c r="K11" s="28">
+      <c r="K11" s="28"/>
+      <c r="L11" s="28">
         <v>10</v>
       </c>
-      <c r="L11" s="28">
+      <c r="M11" s="28">
         <v>12</v>
       </c>
-      <c r="M11" s="28">
+      <c r="N11" s="28">
         <v>19</v>
-      </c>
-      <c r="N11" s="28">
-        <v>25</v>
       </c>
       <c r="O11" s="28">
         <v>25</v>
       </c>
       <c r="P11" s="28">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="28">
         <v>23</v>
       </c>
-      <c r="Q11" s="28">
+      <c r="R11" s="28">
         <v>20</v>
       </c>
-      <c r="R11" s="28">
+      <c r="S11" s="28">
         <v>10</v>
       </c>
-      <c r="S11" s="28">
+      <c r="T11" s="28">
         <v>5</v>
       </c>
-      <c r="T11" s="28">
+      <c r="U11" s="28">
         <v>4</v>
       </c>
-      <c r="U11" s="28"/>
       <c r="V11" s="28"/>
-    </row>
-    <row r="12" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W11" s="28"/>
+    </row>
+    <row r="12" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="19">
         <v>23173</v>
       </c>
@@ -2251,23 +2264,21 @@
         <v>34</v>
       </c>
       <c r="D12" s="19"/>
-      <c r="E12" s="28"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
-      <c r="K12" s="28">
+      <c r="K12" s="28"/>
+      <c r="L12" s="28">
         <v>2</v>
       </c>
-      <c r="L12" s="28">
+      <c r="M12" s="28">
         <v>4</v>
       </c>
-      <c r="M12" s="28">
+      <c r="N12" s="28">
         <v>14</v>
-      </c>
-      <c r="N12" s="28">
-        <v>17</v>
       </c>
       <c r="O12" s="28">
         <v>17</v>
@@ -2276,25 +2287,28 @@
         <v>17</v>
       </c>
       <c r="Q12" s="28">
+        <v>17</v>
+      </c>
+      <c r="R12" s="28">
         <v>12</v>
       </c>
-      <c r="R12" s="28">
+      <c r="S12" s="28">
         <v>7</v>
       </c>
-      <c r="S12" s="28">
+      <c r="T12" s="28">
         <v>5</v>
-      </c>
-      <c r="T12" s="28">
-        <v>3</v>
       </c>
       <c r="U12" s="28">
         <v>3</v>
       </c>
       <c r="V12" s="28">
+        <v>3</v>
+      </c>
+      <c r="W12" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="19">
         <v>23233</v>
       </c>
@@ -2305,48 +2319,49 @@
         <v>34</v>
       </c>
       <c r="D13" s="19"/>
-      <c r="E13" s="28"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
-      <c r="K13" s="28">
+      <c r="K13" s="28"/>
+      <c r="L13" s="28">
         <v>3</v>
       </c>
-      <c r="L13" s="28">
+      <c r="M13" s="28">
         <v>4</v>
       </c>
-      <c r="M13" s="28">
+      <c r="N13" s="28">
         <v>10</v>
       </c>
-      <c r="N13" s="28">
+      <c r="O13" s="28">
         <v>15</v>
       </c>
-      <c r="O13" s="30">
+      <c r="P13" s="30">
         <v>17</v>
       </c>
-      <c r="P13" s="28">
+      <c r="Q13" s="28">
         <v>16</v>
       </c>
-      <c r="Q13" s="28">
+      <c r="R13" s="28">
         <v>14</v>
       </c>
-      <c r="R13" s="28">
+      <c r="S13" s="28">
         <v>7</v>
       </c>
-      <c r="S13" s="28">
+      <c r="T13" s="28">
         <v>5</v>
       </c>
-      <c r="T13" s="28">
+      <c r="U13" s="28">
         <v>3</v>
       </c>
-      <c r="U13" s="28">
+      <c r="V13" s="28">
         <v>1</v>
       </c>
-      <c r="V13" s="28"/>
-    </row>
-    <row r="14" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="W13" s="28"/>
+    </row>
+    <row r="14" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="19">
         <v>23178</v>
       </c>
@@ -2357,44 +2372,45 @@
         <v>34</v>
       </c>
       <c r="D14" s="19"/>
-      <c r="E14" s="28"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
-      <c r="L14" s="28">
+      <c r="L14" s="28"/>
+      <c r="M14" s="28">
         <v>1</v>
       </c>
-      <c r="M14" s="28">
+      <c r="N14" s="28">
         <v>6</v>
       </c>
-      <c r="N14" s="28">
+      <c r="O14" s="28">
         <v>8</v>
       </c>
-      <c r="O14" s="28">
+      <c r="P14" s="28">
         <v>12</v>
       </c>
-      <c r="P14" s="28">
+      <c r="Q14" s="28">
         <v>14</v>
       </c>
-      <c r="Q14" s="28">
+      <c r="R14" s="28">
         <v>12</v>
       </c>
-      <c r="R14" s="28">
+      <c r="S14" s="28">
         <v>8</v>
       </c>
-      <c r="S14" s="28">
+      <c r="T14" s="28">
         <v>6</v>
       </c>
-      <c r="T14" s="28">
+      <c r="U14" s="28">
         <v>5</v>
       </c>
-      <c r="U14" s="28">
+      <c r="V14" s="28">
         <v>3</v>
       </c>
-      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Agregar reference_id y box_id a transacciones de stock (#10)
* upgrade puma.

* add reference_id to stock_transactions (DB only)

* add reference_id  migration

* Add sample reference_id PL.

* Update gitignore

* Actualizamos todas las referencias al nuevo campo "reference_id".

* Agregamos un test cases para reference_id (aun esta en rojo)

* Update comments sobre la estrategia para incorporar reference_id
(Como reemplazar las columnas)

* Actualizamos template parser para que interprete reference_id.
Todos los tests en verde, pero el campo no esta en la columna
"A" sino en la "D".

* Se agrego box_id a las transacciones de stock. (#9)

Add refrence_id y box_id a las transacciones de stock

Co-authored-by: Jonatan <jonatansteckler@hotmail.com>
</commit_message>
<xml_diff>
--- a/test/fixtures/files/mixed-sizes.xlsx
+++ b/test/fixtures/files/mixed-sizes.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiralles/Projects/stash/5411-IM-API/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonatansteckler/dev/stash/5411-IM-API/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A311AA4F-E19F-264B-8A94-4B3322F1294C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6E62FA-B42F-7743-8603-1DEBF9B19DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32140" yWindow="2460" windowWidth="26600" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template Modelo" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja 1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>BOX</t>
   </si>
@@ -181,6 +181,9 @@
   <si>
     <t>34</t>
     <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>REFERENCE_ID</t>
   </si>
 </sst>
 </file>
@@ -567,8 +570,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="3" xr:uid="{A36ED469-7401-3E49-AF43-EA460355A6BD}"/>
   </cellStyles>
@@ -1725,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1736,9 +1739,10 @@
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="5" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>23</v>
       </c>
@@ -1749,61 +1753,67 @@
         <v>2</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="K1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="O1" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="P1" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="32" t="s">
+      <c r="Q1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="R1" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="S1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="32" t="s">
+      <c r="T1" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="U1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="V1" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="32" t="s">
+      <c r="W1" s="32" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="16">
         <v>23694</v>
       </c>
@@ -1813,30 +1823,32 @@
       <c r="C2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
       <c r="O2" s="22"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
-      <c r="R2" s="22">
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22">
         <v>1</v>
       </c>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22">
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="16">
         <v>23695</v>
       </c>
@@ -1846,24 +1858,24 @@
       <c r="C3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="23">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="23">
         <v>7</v>
       </c>
-      <c r="F3" s="21">
+      <c r="H3" s="21">
         <v>14</v>
       </c>
-      <c r="G3" s="21">
+      <c r="I3" s="21">
         <v>11</v>
       </c>
-      <c r="H3" s="21">
+      <c r="J3" s="21">
         <v>8</v>
       </c>
-      <c r="I3" s="21">
+      <c r="K3" s="21">
         <v>2</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
@@ -1874,8 +1886,10 @@
       <c r="S3" s="22"/>
       <c r="T3" s="22"/>
       <c r="U3" s="22"/>
-    </row>
-    <row r="4" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+    </row>
+    <row r="4" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17">
         <v>21370</v>
       </c>
@@ -1891,32 +1905,28 @@
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="21">
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="21">
         <v>8</v>
       </c>
-      <c r="K4" s="21">
+      <c r="M4" s="21">
         <v>11</v>
       </c>
-      <c r="L4" s="21">
+      <c r="N4" s="21">
         <v>18</v>
       </c>
-      <c r="M4" s="21">
+      <c r="O4" s="21">
         <v>21</v>
       </c>
-      <c r="N4" s="21">
+      <c r="P4" s="21">
         <v>24</v>
       </c>
-      <c r="O4" s="21">
+      <c r="Q4" s="21">
         <v>26</v>
       </c>
-      <c r="P4" s="21">
+      <c r="R4" s="21">
         <v>18</v>
-      </c>
-      <c r="Q4" s="21">
-        <v>12</v>
-      </c>
-      <c r="R4" s="21">
-        <v>13</v>
       </c>
       <c r="S4" s="21">
         <v>12</v>
@@ -1924,9 +1934,15 @@
       <c r="T4" s="21">
         <v>13</v>
       </c>
-      <c r="U4" s="21"/>
-    </row>
-    <row r="5" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="U4" s="21">
+        <v>12</v>
+      </c>
+      <c r="V4" s="21">
+        <v>13</v>
+      </c>
+      <c r="W4" s="21"/>
+    </row>
+    <row r="5" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="18">
         <v>20343</v>
       </c>
@@ -1936,30 +1952,32 @@
       <c r="C5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
       <c r="L5" s="24"/>
-      <c r="M5" s="24">
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24">
         <v>1</v>
       </c>
-      <c r="N5" s="24">
+      <c r="P5" s="24">
         <v>1</v>
       </c>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
-    </row>
-    <row r="6" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+    </row>
+    <row r="6" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="18">
         <v>23925</v>
       </c>
@@ -1969,50 +1987,52 @@
       <c r="C6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
-      <c r="J6" s="24">
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="24">
         <v>2</v>
       </c>
-      <c r="K6" s="24">
+      <c r="M6" s="24">
         <v>7</v>
       </c>
-      <c r="L6" s="24">
+      <c r="N6" s="24">
         <v>15</v>
       </c>
-      <c r="M6" s="24">
+      <c r="O6" s="24">
         <v>15</v>
       </c>
-      <c r="N6" s="24">
+      <c r="P6" s="24">
         <v>16</v>
       </c>
-      <c r="O6" s="24">
+      <c r="Q6" s="24">
         <v>16</v>
       </c>
-      <c r="P6" s="24">
+      <c r="R6" s="24">
         <v>12</v>
       </c>
-      <c r="Q6" s="24">
+      <c r="S6" s="24">
         <v>7</v>
       </c>
-      <c r="R6" s="24">
+      <c r="T6" s="24">
         <v>4</v>
       </c>
-      <c r="S6" s="24">
+      <c r="U6" s="24">
         <v>2</v>
       </c>
-      <c r="T6" s="24">
+      <c r="V6" s="24">
         <v>2</v>
       </c>
-      <c r="U6" s="24">
+      <c r="W6" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="18">
         <v>23926</v>
       </c>
@@ -2022,46 +2042,48 @@
       <c r="C7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
-      <c r="J7" s="24">
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="24">
         <v>4</v>
       </c>
-      <c r="K7" s="24">
+      <c r="M7" s="24">
         <v>5</v>
       </c>
-      <c r="L7" s="24">
+      <c r="N7" s="24">
         <v>13</v>
       </c>
-      <c r="M7" s="24">
+      <c r="O7" s="24">
         <v>20</v>
       </c>
-      <c r="N7" s="24">
+      <c r="P7" s="24">
         <v>21</v>
       </c>
-      <c r="O7" s="24">
+      <c r="Q7" s="24">
         <v>21</v>
       </c>
-      <c r="P7" s="24">
+      <c r="R7" s="24">
         <v>19</v>
       </c>
-      <c r="Q7" s="24">
+      <c r="S7" s="24">
         <v>8</v>
       </c>
-      <c r="R7" s="24">
+      <c r="T7" s="24">
         <v>5</v>
       </c>
-      <c r="S7" s="24">
+      <c r="U7" s="24">
         <v>4</v>
       </c>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-    </row>
-    <row r="8" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+    </row>
+    <row r="8" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="18">
         <v>23928</v>
       </c>
@@ -2071,32 +2093,34 @@
       <c r="C8" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24">
-        <v>1</v>
-      </c>
-      <c r="M8" s="24">
-        <v>1</v>
-      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
       <c r="N8" s="24">
         <v>1</v>
       </c>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
+      <c r="O8" s="24">
+        <v>1</v>
+      </c>
+      <c r="P8" s="24">
+        <v>1</v>
+      </c>
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
       <c r="S8" s="24"/>
       <c r="T8" s="24"/>
       <c r="U8" s="24"/>
-    </row>
-    <row r="9" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+    </row>
+    <row r="9" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="19">
         <v>23607</v>
       </c>
@@ -2106,34 +2130,36 @@
       <c r="C9" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27">
-        <v>1</v>
-      </c>
-      <c r="L9" s="27">
-        <v>1</v>
-      </c>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
       <c r="M9" s="27">
         <v>1</v>
       </c>
       <c r="N9" s="27">
         <v>1</v>
       </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
+      <c r="O9" s="27">
+        <v>1</v>
+      </c>
+      <c r="P9" s="27">
+        <v>1</v>
+      </c>
       <c r="Q9" s="27"/>
       <c r="R9" s="27"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="29"/>
-    </row>
-    <row r="10" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="29"/>
+    </row>
+    <row r="10" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="19">
         <v>23180</v>
       </c>
@@ -2143,26 +2169,26 @@
       <c r="C10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="28">
         <v>41</v>
       </c>
-      <c r="E10" s="28">
+      <c r="G10" s="28">
         <v>87</v>
       </c>
-      <c r="F10" s="28">
+      <c r="H10" s="28">
         <v>115</v>
       </c>
-      <c r="G10" s="28">
+      <c r="I10" s="28">
         <v>74</v>
       </c>
-      <c r="H10" s="28">
+      <c r="J10" s="28">
         <v>41</v>
       </c>
-      <c r="I10" s="28">
+      <c r="K10" s="28">
         <v>9</v>
       </c>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -2172,9 +2198,11 @@
       <c r="R10" s="28"/>
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
-      <c r="U10" s="29"/>
-    </row>
-    <row r="11" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="29"/>
+    </row>
+    <row r="11" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="19">
         <v>23608</v>
       </c>
@@ -2184,46 +2212,48 @@
       <c r="C11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
-      <c r="J11" s="28">
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28">
         <v>10</v>
       </c>
-      <c r="K11" s="28">
+      <c r="M11" s="28">
         <v>12</v>
       </c>
-      <c r="L11" s="28">
+      <c r="N11" s="28">
         <v>19</v>
       </c>
-      <c r="M11" s="28">
+      <c r="O11" s="28">
         <v>25</v>
       </c>
-      <c r="N11" s="28">
+      <c r="P11" s="28">
         <v>25</v>
       </c>
-      <c r="O11" s="28">
+      <c r="Q11" s="28">
         <v>23</v>
       </c>
-      <c r="P11" s="28">
+      <c r="R11" s="28">
         <v>20</v>
       </c>
-      <c r="Q11" s="28">
+      <c r="S11" s="28">
         <v>10</v>
       </c>
-      <c r="R11" s="28">
+      <c r="T11" s="28">
         <v>5</v>
       </c>
-      <c r="S11" s="28">
+      <c r="U11" s="28">
         <v>4</v>
       </c>
-      <c r="T11" s="28"/>
-      <c r="U11" s="28"/>
-    </row>
-    <row r="12" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="V11" s="28"/>
+      <c r="W11" s="28"/>
+    </row>
+    <row r="12" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="19">
         <v>23173</v>
       </c>
@@ -2233,50 +2263,52 @@
       <c r="C12" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
-      <c r="J12" s="28">
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28">
         <v>2</v>
       </c>
-      <c r="K12" s="28">
+      <c r="M12" s="28">
         <v>4</v>
       </c>
-      <c r="L12" s="28">
+      <c r="N12" s="28">
         <v>14</v>
-      </c>
-      <c r="M12" s="28">
-        <v>17</v>
-      </c>
-      <c r="N12" s="28">
-        <v>17</v>
       </c>
       <c r="O12" s="28">
         <v>17</v>
       </c>
       <c r="P12" s="28">
+        <v>17</v>
+      </c>
+      <c r="Q12" s="28">
+        <v>17</v>
+      </c>
+      <c r="R12" s="28">
         <v>12</v>
       </c>
-      <c r="Q12" s="28">
+      <c r="S12" s="28">
         <v>7</v>
       </c>
-      <c r="R12" s="28">
+      <c r="T12" s="28">
         <v>5</v>
       </c>
-      <c r="S12" s="28">
+      <c r="U12" s="28">
         <v>3</v>
       </c>
-      <c r="T12" s="28">
+      <c r="V12" s="28">
         <v>3</v>
       </c>
-      <c r="U12" s="28">
+      <c r="W12" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="19">
         <v>23233</v>
       </c>
@@ -2286,48 +2318,50 @@
       <c r="C13" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
-      <c r="J13" s="28">
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28">
         <v>3</v>
       </c>
-      <c r="K13" s="28">
+      <c r="M13" s="28">
         <v>4</v>
       </c>
-      <c r="L13" s="28">
+      <c r="N13" s="28">
         <v>10</v>
       </c>
-      <c r="M13" s="28">
+      <c r="O13" s="28">
         <v>15</v>
       </c>
-      <c r="N13" s="30">
+      <c r="P13" s="30">
         <v>17</v>
       </c>
-      <c r="O13" s="28">
+      <c r="Q13" s="28">
         <v>16</v>
       </c>
-      <c r="P13" s="28">
+      <c r="R13" s="28">
         <v>14</v>
       </c>
-      <c r="Q13" s="28">
+      <c r="S13" s="28">
         <v>7</v>
       </c>
-      <c r="R13" s="28">
+      <c r="T13" s="28">
         <v>5</v>
       </c>
-      <c r="S13" s="28">
+      <c r="U13" s="28">
         <v>3</v>
       </c>
-      <c r="T13" s="28">
+      <c r="V13" s="28">
         <v>1</v>
       </c>
-      <c r="U13" s="28"/>
-    </row>
-    <row r="14" spans="1:21" ht="14" x14ac:dyDescent="0.15">
+      <c r="W13" s="28"/>
+    </row>
+    <row r="14" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="19">
         <v>23178</v>
       </c>
@@ -2337,44 +2371,46 @@
       <c r="C14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
-      <c r="K14" s="28">
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28">
         <v>1</v>
       </c>
-      <c r="L14" s="28">
+      <c r="N14" s="28">
         <v>6</v>
       </c>
-      <c r="M14" s="28">
+      <c r="O14" s="28">
         <v>8</v>
-      </c>
-      <c r="N14" s="28">
-        <v>12</v>
-      </c>
-      <c r="O14" s="28">
-        <v>14</v>
       </c>
       <c r="P14" s="28">
         <v>12</v>
       </c>
       <c r="Q14" s="28">
+        <v>14</v>
+      </c>
+      <c r="R14" s="28">
+        <v>12</v>
+      </c>
+      <c r="S14" s="28">
         <v>8</v>
       </c>
-      <c r="R14" s="28">
+      <c r="T14" s="28">
         <v>6</v>
       </c>
-      <c r="S14" s="28">
+      <c r="U14" s="28">
         <v>5</v>
       </c>
-      <c r="T14" s="28">
+      <c r="V14" s="28">
         <v>3</v>
       </c>
-      <c r="U14" s="26"/>
+      <c r="W14" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>